<commit_message>
added date pulled today
</commit_message>
<xml_diff>
--- a/data/fixtures.xlsx
+++ b/data/fixtures.xlsx
@@ -2334,16 +2334,16 @@
         <v>67</v>
       </c>
       <c r="D65" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="F65" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H65">
         <v>2</v>
       </c>
       <c r="I65">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -2357,16 +2357,16 @@
         <v>67</v>
       </c>
       <c r="D66" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F66" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H66">
         <v>2</v>
       </c>
       <c r="I66">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -2380,16 +2380,16 @@
         <v>67</v>
       </c>
       <c r="D67" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="F67" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="H67">
         <v>2</v>
       </c>
       <c r="I67">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -2400,19 +2400,19 @@
         <v>24</v>
       </c>
       <c r="C68" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D68" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F68" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="H68">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I68">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -2420,22 +2420,22 @@
         <v>7</v>
       </c>
       <c r="B69" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C69" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D69" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F69" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="H69">
         <v>3</v>
       </c>
       <c r="I69">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -2449,13 +2449,13 @@
         <v>69</v>
       </c>
       <c r="D70" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F70" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="H70">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I70">
         <v>4</v>
@@ -2633,16 +2633,16 @@
         <v>68</v>
       </c>
       <c r="D78" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F78" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="H78">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I78">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -2656,10 +2656,10 @@
         <v>69</v>
       </c>
       <c r="D79" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="F79" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H79">
         <v>5</v>
@@ -2679,16 +2679,16 @@
         <v>70</v>
       </c>
       <c r="D80" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="F80" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H80">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I80">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:9">

</xml_diff>